<commit_message>
loading from sidebar; next: saving back
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B559E183-A62B-B848-BFD6-18BF162365BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A7EF7-06A8-AD4F-9913-C7CF412A2077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="500" windowWidth="12160" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="8020" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1211,6 +1211,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1302,7 +1314,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Matthew Turner" refreshedDate="44333.493882407405" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="60" xr:uid="{D02B37FA-6238-8D48-886C-C43B030BE6DB}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:P61" sheet="ArticleStudiesMinimal"/>
+    <worksheetSource ref="B1:P61" sheet="ArticleStudiesMinimal"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="Article" numFmtId="0">
@@ -3140,15 +3152,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
@@ -3161,16 +3173,16 @@
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
     <col min="13" max="13" width="18.6640625" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="42" customWidth="1"/>
     <col min="16" max="16" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>147</v>
@@ -3208,7 +3220,7 @@
       <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="39" t="s">
         <v>115</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -3216,11 +3228,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -3255,7 +3267,7 @@
       <c r="N2" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="40">
         <f>IF(N2, 1, 0)</f>
         <v>1</v>
       </c>
@@ -3264,11 +3276,11 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3303,17 +3315,17 @@
       <c r="N3" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="40">
         <f t="shared" ref="O3:O61" si="1">IF(N3, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -3348,17 +3360,17 @@
       <c r="N4" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -3393,17 +3405,17 @@
       <c r="N5" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -3438,17 +3450,17 @@
       <c r="N6" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -3483,7 +3495,7 @@
       <c r="N7" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3492,11 +3504,11 @@
       </c>
     </row>
     <row r="8" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3531,17 +3543,17 @@
       <c r="N8" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3576,17 +3588,17 @@
       <c r="N9" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3620,17 +3632,17 @@
       <c r="N10" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="41">
         <f t="shared" ref="O10:O11" si="2">IF(N10, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3664,17 +3676,17 @@
       <c r="N11" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="41">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -3709,17 +3721,17 @@
       <c r="N12" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -3754,7 +3766,7 @@
       <c r="N13" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3763,11 +3775,11 @@
       </c>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -3802,17 +3814,17 @@
       <c r="N14" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>23</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
@@ -3850,7 +3862,7 @@
       <c r="N15" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3859,11 +3871,11 @@
       </c>
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="E16" s="11">
         <f>20 * (  ToConvert!C3  / 100)</f>
@@ -3899,7 +3911,7 @@
       <c r="N16" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -3908,11 +3920,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="E17" s="11">
         <f>20 * (  ToConvert!C4  / 100)</f>
@@ -3948,17 +3960,17 @@
       <c r="N17" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>26</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -3996,7 +4008,7 @@
       <c r="N18" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4005,11 +4017,11 @@
       </c>
     </row>
     <row r="19" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
@@ -4047,7 +4059,7 @@
       <c r="N19" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4056,11 +4068,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -4098,17 +4110,17 @@
       <c r="N20" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>29</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -4146,17 +4158,17 @@
       <c r="N21" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>33</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -4194,7 +4206,7 @@
       <c r="N22" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4204,10 +4216,10 @@
     </row>
     <row r="23" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -4245,7 +4257,7 @@
       <c r="N23" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4255,10 +4267,10 @@
     </row>
     <row r="24" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -4296,7 +4308,7 @@
       <c r="N24" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4306,10 +4318,10 @@
     </row>
     <row r="25" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -4347,17 +4359,17 @@
       <c r="N25" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O25" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -4395,17 +4407,17 @@
       <c r="N26" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -4443,7 +4455,7 @@
       <c r="N27" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4453,10 +4465,10 @@
     </row>
     <row r="28" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -4494,17 +4506,17 @@
       <c r="N28" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -4542,17 +4554,17 @@
       <c r="N29" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O29" s="9">
+      <c r="O29" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -4590,17 +4602,17 @@
       <c r="N30" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O30" s="9">
+      <c r="O30" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -4638,17 +4650,17 @@
       <c r="N31" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O31" s="9">
+      <c r="O31" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -4686,17 +4698,17 @@
       <c r="N32" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O32" s="9">
+      <c r="O32" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -4730,7 +4742,7 @@
       <c r="N33" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O33" s="11">
+      <c r="O33" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4740,10 +4752,10 @@
     </row>
     <row r="34" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
@@ -4777,17 +4789,17 @@
       <c r="N34" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O34" s="11">
+      <c r="O34" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -4821,17 +4833,17 @@
       <c r="N35" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O35" s="11">
+      <c r="O35" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
@@ -4865,7 +4877,7 @@
       <c r="N36" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O36" s="11">
+      <c r="O36" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4875,10 +4887,10 @@
     </row>
     <row r="37" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -4912,7 +4924,7 @@
       <c r="N37" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O37" s="11">
+      <c r="O37" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4922,10 +4934,10 @@
     </row>
     <row r="38" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
@@ -4959,7 +4971,7 @@
       <c r="N38" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O38" s="11">
+      <c r="O38" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -4969,10 +4981,10 @@
     </row>
     <row r="39" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -5006,7 +5018,7 @@
       <c r="N39" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O39" s="11">
+      <c r="O39" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5016,10 +5028,10 @@
     </row>
     <row r="40" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -5053,7 +5065,7 @@
       <c r="N40" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O40" s="11">
+      <c r="O40" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5063,10 +5075,10 @@
     </row>
     <row r="41" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -5100,17 +5112,17 @@
       <c r="N41" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O41" s="11">
+      <c r="O41" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
@@ -5144,17 +5156,17 @@
       <c r="N42" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O42" s="11">
+      <c r="O42" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -5189,17 +5201,17 @@
       <c r="N43" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O43" s="9">
+      <c r="O43" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -5234,17 +5246,17 @@
       <c r="N44" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O44" s="9">
+      <c r="O44" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -5279,17 +5291,17 @@
       <c r="N45" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O45" s="9">
+      <c r="O45" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -5324,17 +5336,17 @@
       <c r="N46" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O46" s="9">
+      <c r="O46" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -5369,17 +5381,17 @@
       <c r="N47" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O47" s="9">
+      <c r="O47" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -5414,17 +5426,17 @@
       <c r="N48" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O48" s="9">
+      <c r="O48" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -5459,17 +5471,17 @@
       <c r="N49" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O49" s="9">
+      <c r="O49" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -5504,17 +5516,17 @@
       <c r="N50" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O50" s="9">
+      <c r="O50" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -5549,7 +5561,7 @@
       <c r="N51" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O51" s="9">
+      <c r="O51" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5559,10 +5571,10 @@
     </row>
     <row r="52" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -5596,7 +5608,7 @@
       <c r="N52" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="O52" s="9">
+      <c r="O52" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5606,10 +5618,10 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -5643,17 +5655,17 @@
       <c r="N53" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O53" s="9">
+      <c r="O53" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -5687,7 +5699,7 @@
       <c r="N54" t="b">
         <v>0</v>
       </c>
-      <c r="O54" s="9">
+      <c r="O54" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5697,10 +5709,10 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -5734,17 +5746,17 @@
       <c r="N55" t="b">
         <v>1</v>
       </c>
-      <c r="O55" s="9">
+      <c r="O55" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -5778,7 +5790,7 @@
       <c r="N56" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O56" s="9">
+      <c r="O56" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5788,10 +5800,10 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -5825,17 +5837,17 @@
       <c r="N57" t="b">
         <v>1</v>
       </c>
-      <c r="O57" s="9">
+      <c r="O57" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -5869,17 +5881,17 @@
       <c r="N58" t="b">
         <v>1</v>
       </c>
-      <c r="O58" s="9">
+      <c r="O58" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>88</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -5913,17 +5925,17 @@
       <c r="N59" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="O59" s="9">
+      <c r="O59" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>89</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -5957,17 +5969,17 @@
       <c r="N60" t="b">
         <v>1</v>
       </c>
-      <c r="O60" s="9">
+      <c r="O60" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -6001,7 +6013,7 @@
       <c r="N61" t="b">
         <v>1</v>
       </c>
-      <c r="O61" s="9">
+      <c r="O61" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
need to convert dataframe dtypes
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A7EF7-06A8-AD4F-9913-C7CF412A2077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C05CB1C-4815-0B43-A1D9-3AF41462D9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="8020" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="-11180" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FalseDiscoveryRates" sheetId="11" r:id="rId1"/>
@@ -3153,8 +3153,8 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O1" sqref="O1:O1048576"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
cleaned up print statements; now saving simulation errors
</commit_message>
<xml_diff>
--- a/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
+++ b/GroupPolarizationStatmod/data/CaseStudies_ProtoDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mt/workspace/GroupPolarization/statmod/GroupPolarizationStatmod/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C05CB1C-4815-0B43-A1D9-3AF41462D9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DF4D7D-A274-CB4B-9A9C-71D982C6011F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="-11180" windowWidth="21600" windowHeight="19200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="151">
   <si>
     <t>CaseStudyTag</t>
   </si>
@@ -619,6 +619,12 @@
   </si>
   <si>
     <t>LatentSDPost</t>
+  </si>
+  <si>
+    <t>ObservedMeanPreAbsError</t>
+  </si>
+  <si>
+    <t>ObservedMeanPostAbsError</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1320,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Matthew Turner" refreshedDate="44333.493882407405" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="60" xr:uid="{D02B37FA-6238-8D48-886C-C43B030BE6DB}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:P61" sheet="ArticleStudiesMinimal"/>
+    <worksheetSource ref="B1:R61" sheet="ArticleStudiesMinimal"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="Article" numFmtId="0">
@@ -2346,7 +2352,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A55F5B7-C5FC-0D4E-AD02-78CC73678C7D}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A55F5B7-C5FC-0D4E-AD02-78CC73678C7D}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" showAll="0">
@@ -3150,19 +3156,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P1" sqref="A1:P1"/>
+      <pane xSplit="4" ySplit="20" topLeftCell="K21" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -3170,14 +3178,16 @@
     <col min="9" max="9" width="22.6640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
     <col min="11" max="11" width="25.1640625" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="42" customWidth="1"/>
-    <col min="16" max="16" width="43.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="13" width="26.5" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" style="42" customWidth="1"/>
+    <col min="18" max="18" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>146</v>
       </c>
@@ -3212,22 +3222,28 @@
         <v>91</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="Q1" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
@@ -3258,24 +3274,24 @@
       <c r="K2" s="9">
         <v>0.05</v>
       </c>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-      <c r="M2" s="9">
+      <c r="N2" s="9">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9">
         <v>10</v>
       </c>
-      <c r="N2" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" s="40">
-        <f>IF(N2, 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="40">
+        <f>IF(P2, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -3306,21 +3322,23 @@
       <c r="K3" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L3" s="9">
-        <v>1</v>
-      </c>
-      <c r="M3" s="9">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="O3" s="9">
         <v>10</v>
       </c>
-      <c r="N3" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O3" s="40">
-        <f t="shared" ref="O3:O61" si="1">IF(N3, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="40">
+        <f t="shared" ref="Q3:Q61" si="1">IF(P3, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -3351,21 +3369,23 @@
       <c r="K4" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L4" s="9">
-        <v>1</v>
-      </c>
-      <c r="M4" s="9">
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="9">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9">
         <v>10</v>
       </c>
-      <c r="N4" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O4" s="40">
+      <c r="P4" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
@@ -3396,21 +3416,23 @@
       <c r="K5" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L5" s="9">
-        <v>1</v>
-      </c>
-      <c r="M5" s="9">
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="9">
+        <v>1</v>
+      </c>
+      <c r="O5" s="9">
         <v>10</v>
       </c>
-      <c r="N5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" s="40">
+      <c r="P5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -3441,21 +3463,23 @@
       <c r="K6" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L6" s="9">
-        <v>1</v>
-      </c>
-      <c r="M6" s="9">
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9">
         <v>10</v>
       </c>
-      <c r="N6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O6" s="40">
+      <c r="P6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -3486,24 +3510,24 @@
       <c r="K7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="9">
-        <v>1</v>
-      </c>
-      <c r="M7" s="9">
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+      <c r="O7" s="9">
         <v>10</v>
       </c>
-      <c r="N7" s="9" t="b">
+      <c r="P7" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O7" s="40">
+      <c r="Q7" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="R7" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -3534,21 +3558,23 @@
       <c r="K8" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="11">
         <v>-3</v>
       </c>
-      <c r="M8" s="11">
+      <c r="O8" s="11">
         <v>3</v>
       </c>
-      <c r="N8" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O8" s="41">
+      <c r="P8" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
@@ -3579,21 +3605,23 @@
       <c r="K9" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="11">
         <v>-3</v>
       </c>
-      <c r="M9" s="11">
+      <c r="O9" s="11">
         <v>3</v>
       </c>
-      <c r="N9" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" s="41">
+      <c r="P9" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>119</v>
       </c>
@@ -3623,21 +3651,23 @@
       <c r="K10" s="19">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L10" s="11">
-        <v>1</v>
-      </c>
-      <c r="M10" s="11">
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="11">
+        <v>1</v>
+      </c>
+      <c r="O10" s="11">
         <v>7</v>
       </c>
-      <c r="N10" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O10" s="41">
-        <f t="shared" ref="O10:O11" si="2">IF(N10, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P10" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="41">
+        <f t="shared" ref="Q10:Q11" si="2">IF(P10, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>120</v>
       </c>
@@ -3667,21 +3697,23 @@
       <c r="K11" s="19">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L11" s="11">
-        <v>1</v>
-      </c>
-      <c r="M11" s="11">
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="11">
         <v>7</v>
       </c>
-      <c r="N11" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O11" s="41">
+      <c r="P11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="41">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -3712,21 +3744,23 @@
       <c r="K12" s="18">
         <v>0.01</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="9">
         <v>-9</v>
       </c>
-      <c r="M12" s="9">
+      <c r="O12" s="9">
         <v>9</v>
       </c>
-      <c r="N12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="40">
+      <c r="P12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -3757,24 +3791,24 @@
       <c r="K13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="9">
+      <c r="N13" s="9">
         <v>-9</v>
       </c>
-      <c r="M13" s="9">
+      <c r="O13" s="9">
         <v>9</v>
       </c>
-      <c r="N13" s="9" t="b">
+      <c r="P13" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O13" s="40">
+      <c r="Q13" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="R13" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
@@ -3805,21 +3839,23 @@
       <c r="K14" s="18">
         <v>1E-3</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="9">
         <v>-9</v>
       </c>
-      <c r="M14" s="9">
+      <c r="O14" s="9">
         <v>9</v>
       </c>
-      <c r="N14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="40">
+      <c r="P14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>23</v>
       </c>
@@ -3853,24 +3889,24 @@
       <c r="K15" s="11">
         <v>0.05</v>
       </c>
-      <c r="L15" s="11">
-        <v>1</v>
-      </c>
-      <c r="M15" s="11">
+      <c r="N15" s="11">
+        <v>1</v>
+      </c>
+      <c r="O15" s="11">
         <v>20</v>
       </c>
-      <c r="N15" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15" s="41">
+      <c r="P15" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="R15" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
@@ -3902,24 +3938,24 @@
       <c r="K16" s="11">
         <v>0.05</v>
       </c>
-      <c r="L16" s="11">
-        <v>1</v>
-      </c>
-      <c r="M16" s="11">
+      <c r="N16" s="11">
+        <v>1</v>
+      </c>
+      <c r="O16" s="11">
         <v>20</v>
       </c>
-      <c r="N16" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O16" s="41">
+      <c r="P16" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -3951,21 +3987,23 @@
       <c r="K17" s="19">
         <v>1E-3</v>
       </c>
-      <c r="L17" s="11">
-        <v>1</v>
-      </c>
-      <c r="M17" s="11">
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="11">
+        <v>1</v>
+      </c>
+      <c r="O17" s="11">
         <v>20</v>
       </c>
-      <c r="N17" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O17" s="41">
+      <c r="P17" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>26</v>
       </c>
@@ -3999,24 +4037,24 @@
       <c r="K18" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="11">
-        <v>1</v>
-      </c>
-      <c r="M18" s="11">
+      <c r="N18" s="11">
+        <v>1</v>
+      </c>
+      <c r="O18" s="11">
         <v>20</v>
       </c>
-      <c r="N18" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O18" s="41">
+      <c r="P18" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="R18" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>27</v>
       </c>
@@ -4050,24 +4088,24 @@
       <c r="K19" s="11">
         <v>0.05</v>
       </c>
-      <c r="L19" s="11">
-        <v>1</v>
-      </c>
-      <c r="M19" s="11">
+      <c r="N19" s="11">
+        <v>1</v>
+      </c>
+      <c r="O19" s="11">
         <v>20</v>
       </c>
-      <c r="N19" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" s="41">
+      <c r="P19" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="R19" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>28</v>
       </c>
@@ -4101,21 +4139,23 @@
       <c r="K20" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L20" s="11">
-        <v>1</v>
-      </c>
-      <c r="M20" s="11">
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="11">
+        <v>1</v>
+      </c>
+      <c r="O20" s="11">
         <v>20</v>
       </c>
-      <c r="N20" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20" s="41">
+      <c r="P20" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
@@ -4149,21 +4189,23 @@
       <c r="K21" s="19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L21" s="11">
-        <v>1</v>
-      </c>
-      <c r="M21" s="11">
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="11">
+        <v>1</v>
+      </c>
+      <c r="O21" s="11">
         <v>20</v>
       </c>
-      <c r="N21" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O21" s="41">
+      <c r="P21" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>33</v>
       </c>
@@ -4197,24 +4239,26 @@
       <c r="K22" s="19">
         <v>0.05</v>
       </c>
-      <c r="L22" s="11">
-        <v>1</v>
-      </c>
-      <c r="M22" s="11">
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="11">
+        <v>1</v>
+      </c>
+      <c r="O22" s="11">
         <v>20</v>
       </c>
-      <c r="N22" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O22" s="41">
+      <c r="P22" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P22" s="11" t="s">
+      <c r="R22" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>36</v>
       </c>
@@ -4248,24 +4292,26 @@
       <c r="K23" s="18">
         <v>0.05</v>
       </c>
-      <c r="L23" s="9">
-        <v>1</v>
-      </c>
-      <c r="M23" s="9">
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="9">
+        <v>1</v>
+      </c>
+      <c r="O23" s="9">
         <v>10</v>
       </c>
-      <c r="N23" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O23" s="40">
+      <c r="P23" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="R23" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>37</v>
       </c>
@@ -4299,24 +4345,24 @@
       <c r="K24" s="9">
         <v>0.05</v>
       </c>
-      <c r="L24" s="9">
-        <v>1</v>
-      </c>
-      <c r="M24" s="9">
+      <c r="N24" s="9">
+        <v>1</v>
+      </c>
+      <c r="O24" s="9">
         <v>10</v>
       </c>
-      <c r="N24" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O24" s="40">
+      <c r="P24" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P24" s="9" t="s">
+      <c r="R24" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>38</v>
       </c>
@@ -4350,21 +4396,23 @@
       <c r="K25" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L25" s="9">
-        <v>1</v>
-      </c>
-      <c r="M25" s="9">
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="9">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9">
         <v>10</v>
       </c>
-      <c r="N25" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O25" s="40">
+      <c r="P25" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>39</v>
       </c>
@@ -4398,21 +4446,23 @@
       <c r="K26" s="18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L26" s="9">
-        <v>1</v>
-      </c>
-      <c r="M26" s="9">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="9">
+        <v>1</v>
+      </c>
+      <c r="O26" s="9">
         <v>10</v>
       </c>
-      <c r="N26" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O26" s="40">
+      <c r="P26" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>40</v>
       </c>
@@ -4446,24 +4496,24 @@
       <c r="K27" s="9">
         <v>0.05</v>
       </c>
-      <c r="L27" s="9">
-        <v>1</v>
-      </c>
-      <c r="M27" s="9">
+      <c r="N27" s="9">
+        <v>1</v>
+      </c>
+      <c r="O27" s="9">
         <v>10</v>
       </c>
-      <c r="N27" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O27" s="40">
+      <c r="P27" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P27" s="9" t="s">
+      <c r="R27" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>41</v>
       </c>
@@ -4497,21 +4547,21 @@
       <c r="K28" s="9">
         <v>0.05</v>
       </c>
-      <c r="L28" s="9">
-        <v>1</v>
-      </c>
-      <c r="M28" s="9">
+      <c r="N28" s="9">
+        <v>1</v>
+      </c>
+      <c r="O28" s="9">
         <v>10</v>
       </c>
-      <c r="N28" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O28" s="40">
+      <c r="P28" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>42</v>
       </c>
@@ -4545,21 +4595,21 @@
       <c r="K29" s="9">
         <v>0.05</v>
       </c>
-      <c r="L29" s="9">
-        <v>1</v>
-      </c>
-      <c r="M29" s="9">
+      <c r="N29" s="9">
+        <v>1</v>
+      </c>
+      <c r="O29" s="9">
         <v>10</v>
       </c>
-      <c r="N29" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O29" s="40">
+      <c r="P29" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
@@ -4593,21 +4643,21 @@
       <c r="K30" s="9">
         <v>0.05</v>
       </c>
-      <c r="L30" s="9">
-        <v>1</v>
-      </c>
-      <c r="M30" s="9">
+      <c r="N30" s="9">
+        <v>1</v>
+      </c>
+      <c r="O30" s="9">
         <v>10</v>
       </c>
-      <c r="N30" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O30" s="40">
+      <c r="P30" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>44</v>
       </c>
@@ -4641,21 +4691,21 @@
       <c r="K31" s="9">
         <v>0.05</v>
       </c>
-      <c r="L31" s="9">
-        <v>1</v>
-      </c>
-      <c r="M31" s="9">
+      <c r="N31" s="9">
+        <v>1</v>
+      </c>
+      <c r="O31" s="9">
         <v>10</v>
       </c>
-      <c r="N31" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O31" s="40">
+      <c r="P31" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>45</v>
       </c>
@@ -4689,21 +4739,21 @@
       <c r="K32" s="9">
         <v>0.05</v>
       </c>
-      <c r="L32" s="9">
-        <v>1</v>
-      </c>
-      <c r="M32" s="9">
+      <c r="N32" s="9">
+        <v>1</v>
+      </c>
+      <c r="O32" s="9">
         <v>10</v>
       </c>
-      <c r="N32" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O32" s="40">
+      <c r="P32" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>47</v>
       </c>
@@ -4733,24 +4783,24 @@
       <c r="K33" s="11">
         <v>0.1</v>
       </c>
-      <c r="L33" s="11">
+      <c r="N33" s="11">
         <v>-4</v>
       </c>
-      <c r="M33" s="11">
+      <c r="O33" s="11">
         <v>4</v>
       </c>
-      <c r="N33" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O33" s="41">
+      <c r="P33" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P33" s="11" t="s">
+      <c r="R33" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>48</v>
       </c>
@@ -4780,21 +4830,21 @@
       <c r="K34" s="11">
         <v>0.05</v>
       </c>
-      <c r="L34" s="11">
+      <c r="N34" s="11">
         <v>-4</v>
       </c>
-      <c r="M34" s="11">
+      <c r="O34" s="11">
         <v>4</v>
       </c>
-      <c r="N34" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O34" s="41">
+      <c r="P34" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>49</v>
       </c>
@@ -4824,21 +4874,21 @@
       <c r="K35" s="11">
         <v>0.05</v>
       </c>
-      <c r="L35" s="11">
+      <c r="N35" s="11">
         <v>-4</v>
       </c>
-      <c r="M35" s="11">
+      <c r="O35" s="11">
         <v>4</v>
       </c>
-      <c r="N35" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O35" s="41">
+      <c r="P35" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>50</v>
       </c>
@@ -4868,24 +4918,24 @@
       <c r="K36" s="11">
         <v>0.05</v>
       </c>
-      <c r="L36" s="11">
+      <c r="N36" s="11">
         <v>-4</v>
       </c>
-      <c r="M36" s="11">
+      <c r="O36" s="11">
         <v>4</v>
       </c>
-      <c r="N36" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O36" s="41">
+      <c r="P36" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P36" s="11" t="s">
+      <c r="R36" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>51</v>
       </c>
@@ -4915,24 +4965,24 @@
       <c r="K37" s="11">
         <v>0.05</v>
       </c>
-      <c r="L37" s="11">
+      <c r="N37" s="11">
         <v>-4</v>
       </c>
-      <c r="M37" s="11">
+      <c r="O37" s="11">
         <v>4</v>
       </c>
-      <c r="N37" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O37" s="41">
+      <c r="P37" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P37" s="11" t="s">
+      <c r="R37" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>52</v>
       </c>
@@ -4962,24 +5012,24 @@
       <c r="K38" s="11">
         <v>0.05</v>
       </c>
-      <c r="L38" s="11">
+      <c r="N38" s="11">
         <v>-4</v>
       </c>
-      <c r="M38" s="11">
+      <c r="O38" s="11">
         <v>4</v>
       </c>
-      <c r="N38" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O38" s="41">
+      <c r="P38" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P38" s="11" t="s">
+      <c r="R38" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>53</v>
       </c>
@@ -5009,24 +5059,24 @@
       <c r="K39" s="11">
         <v>0.05</v>
       </c>
-      <c r="L39" s="11">
+      <c r="N39" s="11">
         <v>-4</v>
       </c>
-      <c r="M39" s="11">
+      <c r="O39" s="11">
         <v>4</v>
       </c>
-      <c r="N39" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O39" s="41">
+      <c r="P39" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P39" s="11" t="s">
+      <c r="R39" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>54</v>
       </c>
@@ -5056,24 +5106,24 @@
       <c r="K40" s="11">
         <v>0.01</v>
       </c>
-      <c r="L40" s="11">
+      <c r="N40" s="11">
         <v>-4</v>
       </c>
-      <c r="M40" s="11">
+      <c r="O40" s="11">
         <v>4</v>
       </c>
-      <c r="N40" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O40" s="41">
+      <c r="P40" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P40" s="11" t="s">
+      <c r="R40" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>55</v>
       </c>
@@ -5103,21 +5153,21 @@
       <c r="K41" s="11">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L41" s="11">
+      <c r="N41" s="11">
         <v>-4</v>
       </c>
-      <c r="M41" s="11">
+      <c r="O41" s="11">
         <v>4</v>
       </c>
-      <c r="N41" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O41" s="41">
+      <c r="P41" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>56</v>
       </c>
@@ -5147,21 +5197,21 @@
       <c r="K42" s="11">
         <v>0.05</v>
       </c>
-      <c r="L42" s="11">
+      <c r="N42" s="11">
         <v>-4</v>
       </c>
-      <c r="M42" s="11">
+      <c r="O42" s="11">
         <v>4</v>
       </c>
-      <c r="N42" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O42" s="41">
+      <c r="P42" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>60</v>
       </c>
@@ -5192,21 +5242,21 @@
       <c r="K43" s="9">
         <v>0.01</v>
       </c>
-      <c r="L43" s="9">
+      <c r="N43" s="9">
         <v>-5</v>
       </c>
-      <c r="M43" s="9">
+      <c r="O43" s="9">
         <v>5</v>
       </c>
-      <c r="N43" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O43" s="40">
+      <c r="P43" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>61</v>
       </c>
@@ -5237,21 +5287,21 @@
       <c r="K44" s="9">
         <v>0.01</v>
       </c>
-      <c r="L44" s="9">
+      <c r="N44" s="9">
         <v>-5</v>
       </c>
-      <c r="M44" s="9">
+      <c r="O44" s="9">
         <v>5</v>
       </c>
-      <c r="N44" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O44" s="40">
+      <c r="P44" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>59</v>
       </c>
@@ -5282,21 +5332,21 @@
       <c r="K45" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L45" s="9">
+      <c r="N45" s="9">
         <v>-5</v>
       </c>
-      <c r="M45" s="9">
+      <c r="O45" s="9">
         <v>5</v>
       </c>
-      <c r="N45" s="9" t="b">
+      <c r="P45" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="O45" s="40">
+      <c r="Q45" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>62</v>
       </c>
@@ -5327,21 +5377,21 @@
       <c r="K46" s="9">
         <v>0.01</v>
       </c>
-      <c r="L46" s="9">
+      <c r="N46" s="9">
         <v>-5</v>
       </c>
-      <c r="M46" s="9">
+      <c r="O46" s="9">
         <v>5</v>
       </c>
-      <c r="N46" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O46" s="40">
+      <c r="P46" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>64</v>
       </c>
@@ -5372,21 +5422,21 @@
       <c r="K47" s="9">
         <v>0.05</v>
       </c>
-      <c r="L47" s="9">
+      <c r="N47" s="9">
         <v>-5</v>
       </c>
-      <c r="M47" s="9">
+      <c r="O47" s="9">
         <v>5</v>
       </c>
-      <c r="N47" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O47" s="40">
+      <c r="P47" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>63</v>
       </c>
@@ -5417,21 +5467,21 @@
       <c r="K48" s="9">
         <v>0.01</v>
       </c>
-      <c r="L48" s="9">
+      <c r="N48" s="9">
         <v>-5</v>
       </c>
-      <c r="M48" s="9">
+      <c r="O48" s="9">
         <v>5</v>
       </c>
-      <c r="N48" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O48" s="40">
+      <c r="P48" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>65</v>
       </c>
@@ -5462,21 +5512,21 @@
       <c r="K49" s="9">
         <v>1E-4</v>
       </c>
-      <c r="L49" s="9">
+      <c r="N49" s="9">
         <v>-5</v>
       </c>
-      <c r="M49" s="9">
+      <c r="O49" s="9">
         <v>5</v>
       </c>
-      <c r="N49" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O49" s="40">
+      <c r="P49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>66</v>
       </c>
@@ -5507,21 +5557,21 @@
       <c r="K50" s="9">
         <v>0.01</v>
       </c>
-      <c r="L50" s="9">
+      <c r="N50" s="9">
         <v>-5</v>
       </c>
-      <c r="M50" s="9">
+      <c r="O50" s="9">
         <v>5</v>
       </c>
-      <c r="N50" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O50" s="40">
+      <c r="P50" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>67</v>
       </c>
@@ -5552,24 +5602,24 @@
       <c r="K51" s="9">
         <v>0.01</v>
       </c>
-      <c r="L51" s="9">
+      <c r="N51" s="9">
         <v>-5</v>
       </c>
-      <c r="M51" s="9">
+      <c r="O51" s="9">
         <v>5</v>
       </c>
-      <c r="N51" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O51" s="40">
+      <c r="P51" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P51" s="9" t="s">
+      <c r="R51" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>76</v>
       </c>
@@ -5599,24 +5649,24 @@
       <c r="K52" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L52" s="11">
+      <c r="N52" s="11">
         <v>0</v>
       </c>
-      <c r="M52" s="11">
+      <c r="O52" s="11">
         <v>10</v>
       </c>
-      <c r="N52" s="11" t="b">
+      <c r="P52" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="O52" s="40">
+      <c r="Q52" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P52" s="11" t="s">
+      <c r="R52" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>77</v>
       </c>
@@ -5646,21 +5696,23 @@
       <c r="K53" s="20">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L53" s="11">
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="11">
         <v>0</v>
       </c>
-      <c r="M53" s="11">
+      <c r="O53" s="11">
         <v>10</v>
       </c>
-      <c r="N53" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O53" s="40">
+      <c r="P53" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>78</v>
       </c>
@@ -5690,24 +5742,24 @@
       <c r="K54" t="s">
         <v>30</v>
       </c>
-      <c r="L54" s="11">
+      <c r="N54" s="11">
         <v>-3</v>
       </c>
-      <c r="M54" s="11">
+      <c r="O54" s="11">
         <v>3</v>
       </c>
-      <c r="N54" t="b">
+      <c r="P54" t="b">
         <v>0</v>
       </c>
-      <c r="O54" s="40">
+      <c r="Q54" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P54" t="s">
+      <c r="R54" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>79</v>
       </c>
@@ -5737,21 +5789,21 @@
       <c r="K55">
         <v>1E-3</v>
       </c>
-      <c r="L55" s="11">
+      <c r="N55" s="11">
         <v>-3</v>
       </c>
-      <c r="M55" s="11">
+      <c r="O55" s="11">
         <v>3</v>
       </c>
-      <c r="N55" t="b">
-        <v>1</v>
-      </c>
-      <c r="O55" s="40">
+      <c r="P55" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>82</v>
       </c>
@@ -5781,24 +5833,26 @@
       <c r="K56" s="18">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="L56" s="9">
-        <v>1</v>
-      </c>
-      <c r="M56" s="9">
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="9">
+        <v>1</v>
+      </c>
+      <c r="O56" s="9">
         <v>10</v>
       </c>
-      <c r="N56" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56" s="40">
+      <c r="P56" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P56" s="9" t="s">
+      <c r="R56" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>87</v>
       </c>
@@ -5828,21 +5882,21 @@
       <c r="K57">
         <v>0.05</v>
       </c>
-      <c r="L57" s="11">
-        <v>1</v>
-      </c>
-      <c r="M57" s="11">
+      <c r="N57" s="11">
+        <v>1</v>
+      </c>
+      <c r="O57" s="11">
         <v>10</v>
       </c>
-      <c r="N57" t="b">
-        <v>1</v>
-      </c>
-      <c r="O57" s="40">
+      <c r="P57" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>86</v>
       </c>
@@ -5872,21 +5926,21 @@
       <c r="K58">
         <v>1E-3</v>
       </c>
-      <c r="L58" s="11">
-        <v>1</v>
-      </c>
-      <c r="M58" s="11">
+      <c r="N58" s="11">
+        <v>1</v>
+      </c>
+      <c r="O58" s="11">
         <v>10</v>
       </c>
-      <c r="N58" t="b">
-        <v>1</v>
-      </c>
-      <c r="O58" s="40">
+      <c r="P58" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>88</v>
       </c>
@@ -5916,21 +5970,21 @@
       <c r="K59">
         <v>0.01</v>
       </c>
-      <c r="L59" s="11">
-        <v>1</v>
-      </c>
-      <c r="M59" s="11">
+      <c r="N59" s="11">
+        <v>1</v>
+      </c>
+      <c r="O59" s="11">
         <v>10</v>
       </c>
-      <c r="N59" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="O59" s="40">
+      <c r="P59" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>89</v>
       </c>
@@ -5960,21 +6014,21 @@
       <c r="K60">
         <v>0.01</v>
       </c>
-      <c r="L60" s="11">
-        <v>1</v>
-      </c>
-      <c r="M60" s="11">
+      <c r="N60" s="11">
+        <v>1</v>
+      </c>
+      <c r="O60" s="11">
         <v>10</v>
       </c>
-      <c r="N60" t="b">
-        <v>1</v>
-      </c>
-      <c r="O60" s="40">
+      <c r="P60" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>90</v>
       </c>
@@ -6004,21 +6058,21 @@
       <c r="K61">
         <v>0.01</v>
       </c>
-      <c r="L61" s="11">
-        <v>1</v>
-      </c>
-      <c r="M61" s="11">
+      <c r="N61" s="11">
+        <v>1</v>
+      </c>
+      <c r="O61" s="11">
         <v>10</v>
       </c>
-      <c r="N61" t="b">
-        <v>1</v>
-      </c>
-      <c r="O61" s="40">
+      <c r="P61" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="40">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G63" s="37"/>
       <c r="H63" s="38"/>
     </row>

</xml_diff>